<commit_message>
Included Formats, print stmts for visibility and corrected date/time column values
</commit_message>
<xml_diff>
--- a/source_dir/productManual.xlsx
+++ b/source_dir/productManual.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\The Volt\script\saleChannelWorkings\amazonWorkings\amazonOrderReport\source_dir\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819174A4-9E62-4A4D-9D0E-75F2F8B30D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1711,8 +1717,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1775,13 +1781,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1819,7 +1833,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1853,6 +1867,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1887,9 +1902,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2062,14 +2078,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2127,7 +2157,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2186,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2185,7 +2215,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2214,7 +2244,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2243,7 +2273,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2272,7 +2302,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2301,7 +2331,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2330,7 +2360,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2389,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2388,7 +2418,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2417,7 +2447,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2476,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2475,7 +2505,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2504,7 +2534,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2533,7 +2563,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2562,7 +2592,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2576,7 +2606,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2590,7 +2620,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2613,7 +2643,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2639,7 +2669,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2665,7 +2695,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2691,7 +2721,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2717,7 +2747,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2743,7 +2773,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2769,7 +2799,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2795,7 +2825,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2821,7 +2851,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2847,7 +2877,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2873,7 +2903,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2902,7 +2932,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2922,7 +2952,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2936,7 +2966,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2953,7 +2983,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2976,7 +3006,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2993,7 +3023,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -3007,7 +3037,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -3030,7 +3060,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -3053,7 +3083,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3076,7 +3106,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -3099,7 +3129,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -3122,7 +3152,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -3145,7 +3175,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -3162,7 +3192,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -3185,7 +3215,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -3202,7 +3232,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -3213,7 +3243,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -3242,7 +3272,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -3271,7 +3301,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -3300,7 +3330,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -3326,7 +3356,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -3352,7 +3382,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -3372,7 +3402,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -3398,7 +3428,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -3424,7 +3454,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -3450,7 +3480,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -3473,7 +3503,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -3496,7 +3526,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -3519,7 +3549,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3545,7 +3575,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3562,7 +3592,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -3585,7 +3615,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -3608,7 +3638,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -3637,7 +3667,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -3654,7 +3684,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -3680,7 +3710,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -3709,7 +3739,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -3732,7 +3762,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -3755,7 +3785,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3769,7 +3799,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -3786,7 +3816,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -3812,7 +3842,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -3835,7 +3865,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -3849,7 +3879,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -3866,7 +3896,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -3889,7 +3919,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -3912,7 +3942,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -3935,7 +3965,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -3958,7 +3988,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -3984,7 +4014,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -4001,7 +4031,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -4018,7 +4048,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -4035,7 +4065,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -4052,7 +4082,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -4069,7 +4099,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -4089,7 +4119,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -4106,7 +4136,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -4123,7 +4153,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -4140,7 +4170,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -4163,7 +4193,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>

</xml_diff>